<commit_message>
updated documentation and fixed an unauthorized change someone made to the excel file
</commit_message>
<xml_diff>
--- a/data/MultiSheetBrickData.xlsx
+++ b/data/MultiSheetBrickData.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -10212,13 +10212,13 @@
     <t>2 North</t>
   </si>
   <si>
-    <t>AnnieRoseberry</t>
+    <t>Annie Roseberry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
@@ -10773,8 +10773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -10834,9 +10834,7 @@
       <c r="G2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="37">
-        <v>1</v>
-      </c>
+      <c r="H2" s="37"/>
       <c r="I2" s="36"/>
       <c r="J2" s="37"/>
     </row>
@@ -18226,8 +18224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M374"/>
   <sheetViews>
-    <sheetView topLeftCell="A383" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changed one cell type in data file
</commit_message>
<xml_diff>
--- a/data/MultiSheetBrickData.xlsx
+++ b/data/MultiSheetBrickData.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bricks" sheetId="1" r:id="rId1"/>
@@ -10218,7 +10218,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
@@ -10773,8 +10773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U289"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -18224,8 +18224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M374"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Trying to fix ONE cell type
</commit_message>
<xml_diff>
--- a/data/MultiSheetBrickData.xlsx
+++ b/data/MultiSheetBrickData.xlsx
@@ -481,7 +481,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3501" uniqueCount="2670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3502" uniqueCount="2671">
   <si>
     <t>Personalization</t>
   </si>
@@ -10213,6 +10213,9 @@
   </si>
   <si>
     <t>Annie Roseberry</t>
+  </si>
+  <si>
+    <t>10/1/2011</t>
   </si>
 </sst>
 </file>
@@ -10377,7 +10380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -10489,6 +10492,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -18352,8 +18358,8 @@
       <c r="D4" s="37">
         <v>4</v>
       </c>
-      <c r="E4" s="13">
-        <v>40817</v>
+      <c r="E4" s="38" t="s">
+        <v>2670</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>1291</v>

</xml_diff>

<commit_message>
one final excel change
</commit_message>
<xml_diff>
--- a/data/MultiSheetBrickData.xlsx
+++ b/data/MultiSheetBrickData.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6D4BCB-CDD0-45EB-AE5E-F146CCCA4E9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bricks" sheetId="1" r:id="rId1"/>
@@ -21,12 +20,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="F16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E40" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="E40" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E58" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="E58" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -100,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G64" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="G64" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G94" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="G94" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -149,7 +148,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F131" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="F131" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -173,7 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F212" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="F212" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -198,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E237" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="E237" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -227,12 +226,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="F10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -257,7 +256,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="G18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -282,7 +281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F115" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="F115" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -307,7 +306,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I124" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="I124" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -332,7 +331,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F144" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="F144" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -356,7 +355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H144" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
+    <comment ref="H144" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -380,7 +379,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H168" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
+    <comment ref="H168" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -405,7 +404,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G206" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
+    <comment ref="G206" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -429,7 +428,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F210" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
+    <comment ref="F210" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -453,7 +452,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J210" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
+    <comment ref="J210" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -10225,7 +10224,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
@@ -10384,7 +10383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -10496,9 +10495,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -10780,11 +10776,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U289"/>
   <sheetViews>
-    <sheetView topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="A264" sqref="A264"/>
+    <sheetView topLeftCell="A256" workbookViewId="0">
+      <selection activeCell="A260" sqref="A260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -18231,11 +18227,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M374"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="F120" sqref="F120:I120"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="H165" sqref="H165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23299,7 +23295,7 @@
       <c r="G165" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H165" s="38" t="s">
+      <c r="H165" s="37" t="s">
         <v>2671</v>
       </c>
       <c r="L165" s="33"/>

</xml_diff>